<commit_message>
Dashboard Page shows the latest playlists
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9F1A6C1-DB4E-4B04-83E7-6B55951C075A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C654E70-250D-4653-87CC-D153BFFD4BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="1710" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Visualizer Add-in" sheetId="20" r:id="rId1"/>
     <sheet name="Etape" sheetId="22" r:id="rId2"/>
-    <sheet name="Getting Started" sheetId="21" r:id="rId3"/>
-    <sheet name="Understanding Diagram Data" sheetId="11" r:id="rId4"/>
-    <sheet name="Shape Notation Mapping" sheetId="13" state="hidden" r:id="rId5"/>
+    <sheet name="Bad Links" sheetId="23" r:id="rId3"/>
+    <sheet name="Getting Started" sheetId="21" r:id="rId4"/>
+    <sheet name="Understanding Diagram Data" sheetId="11" r:id="rId5"/>
+    <sheet name="Shape Notation Mapping" sheetId="13" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="ShapeNotation" localSheetId="4">'Shape Notation Mapping'!$A$2:$A$16</definedName>
+    <definedName name="ShapeNotation" localSheetId="5">'Shape Notation Mapping'!$A$2:$A$16</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Organization Chart - Data Visualizer Add-in</t>
   </si>
@@ -276,13 +277,22 @@
   </si>
   <si>
     <t>creaza articol nou in playlist</t>
+  </si>
+  <si>
+    <t>Adaugator</t>
+  </si>
+  <si>
+    <t>Feature: in setari se poate indica la ce ore se incepe Playlistul</t>
+  </si>
+  <si>
+    <t>https://www.magnetic-it.com/wp-content/uploads/2022/04/power-metter.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,14 +667,14 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Header_LineFill" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -679,9 +689,6 @@
   <dxfs count="10">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -697,6 +704,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2175,7 +2185,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{655CCE42-40DB-48C4-AADF-036FE2C664DE}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{655CCE42-40DB-48C4-AADF-036FE2C664DE}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E8" xr:uid="{655CCE42-40DB-48C4-AADF-036FE2C664DE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2184,11 +2194,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3E7B9233-AE98-474D-B876-BCE1CF4D0595}" name="Employee ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{6BCE90F5-3437-4034-91B2-364F1868DF5D}" name="Name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{B16C0A6F-259F-4390-8728-56A2EF86EDEA}" name="Title" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A54D00B3-72EA-4E1F-BCCF-77834BF63D17}" name="Manager ID" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{07D59069-3E84-45BB-B86A-C124BBA635D2}" name="Role Type" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{3E7B9233-AE98-474D-B876-BCE1CF4D0595}" name="Employee ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6BCE90F5-3437-4034-91B2-364F1868DF5D}" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B16C0A6F-259F-4390-8728-56A2EF86EDEA}" name="Title" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A54D00B3-72EA-4E1F-BCCF-77834BF63D17}" name="Manager ID" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{07D59069-3E84-45BB-B86A-C124BBA635D2}" name="Role Type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="ProcessMapTable" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2528,132 +2538,132 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2679,25 +2689,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBDDE4C-EB2B-4BBA-859C-D0E9535D6E70}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="B3">
         <v>1</v>
       </c>
@@ -2710,16 +2720,22 @@
       <c r="E3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="D4" t="s">
         <v>65</v>
       </c>
       <c r="E4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="D5" t="s">
         <v>67</v>
       </c>
@@ -2727,7 +2743,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="D6" t="s">
         <v>69</v>
       </c>
@@ -2735,7 +2751,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="D7" t="s">
         <v>71</v>
       </c>
@@ -2743,7 +2759,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="B9">
         <v>2</v>
       </c>
@@ -2757,7 +2773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="D10" t="s">
         <v>69</v>
       </c>
@@ -2765,7 +2781,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="D11" t="s">
         <v>77</v>
       </c>
@@ -2779,6 +2795,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CDC44D-8D80-47B8-B351-C113B78A37AD}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="73.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36287276-1A1B-174E-942F-85F8F1AB748F}">
   <sheetPr>
     <tabColor rgb="FF217346"/>
@@ -2789,27 +2828,27 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="59.44140625" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="58.6640625" customWidth="1"/>
-    <col min="10" max="10" width="4.109375" customWidth="1"/>
-    <col min="11" max="11" width="75.109375" customWidth="1"/>
-    <col min="12" max="12" width="49.33203125" customWidth="1"/>
+    <col min="9" max="9" width="58.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="75.140625" customWidth="1"/>
+    <col min="12" max="12" width="49.28515625" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="8.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A1" s="38"/>
-      <c r="B1" s="38"/>
+    <row r="1" spans="1:58">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
@@ -2867,7 +2906,7 @@
       <c r="BE1" s="25"/>
       <c r="BF1" s="25"/>
     </row>
-    <row r="2" spans="1:58" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" ht="40.5">
       <c r="A2" s="19"/>
       <c r="B2" s="19"/>
       <c r="C2" s="26" t="s">
@@ -2929,7 +2968,7 @@
       <c r="BE2" s="19"/>
       <c r="BF2" s="19"/>
     </row>
-    <row r="3" spans="1:58" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" ht="30" customHeight="1">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="27" t="s">
@@ -2991,11 +3030,11 @@
       <c r="BE3" s="19"/>
       <c r="BF3" s="19"/>
     </row>
-    <row r="19" spans="1:23" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="38.25" customHeight="1">
       <c r="G19" s="9"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:23" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="38.25">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="20" t="s">
@@ -3014,7 +3053,7 @@
       </c>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" spans="1:23" ht="27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="40.5">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="30" t="s">
@@ -3028,11 +3067,11 @@
       <c r="I21" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="39" t="s">
+      <c r="K21" s="41" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="99" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="37" t="s">
@@ -3046,9 +3085,9 @@
       <c r="I22" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K22" s="41"/>
+    </row>
+    <row r="23" spans="1:23" ht="15.75">
       <c r="C23" s="35" t="s">
         <v>34</v>
       </c>
@@ -3056,7 +3095,7 @@
       <c r="I23" s="34"/>
       <c r="K23" s="34"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23">
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
       <c r="R24" s="23"/>
@@ -3066,7 +3105,7 @@
       <c r="V24" s="23"/>
       <c r="W24" s="23"/>
     </row>
-    <row r="25" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="27" customHeight="1">
       <c r="C25" s="24"/>
       <c r="I25" s="24"/>
       <c r="P25" s="23"/>
@@ -3078,7 +3117,7 @@
       <c r="V25" s="23"/>
       <c r="W25" s="23"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23">
       <c r="C26" s="24"/>
       <c r="P26" s="23"/>
       <c r="Q26" s="23"/>
@@ -3089,7 +3128,7 @@
       <c r="V26" s="23"/>
       <c r="W26" s="23"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23">
       <c r="P27" s="23"/>
       <c r="Q27" s="23"/>
       <c r="R27" s="23"/>
@@ -3114,7 +3153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF217346"/>
@@ -3123,21 +3162,21 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="15" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:73" s="15" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -3212,86 +3251,86 @@
       <c r="BT1" s="29"/>
       <c r="BU1" s="29"/>
     </row>
-    <row r="2" spans="1:73" s="7" customFormat="1" ht="40.35" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:73" s="7" customFormat="1" ht="40.35" customHeight="1" thickTop="1">
       <c r="B2" s="32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:73" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:73" s="8" customFormat="1" ht="30" customHeight="1">
       <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:73" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:73" ht="15" customHeight="1"/>
+    <row r="5" spans="1:73" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:73" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:73" ht="60" customHeight="1">
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:73" ht="19.2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:73" ht="17.25">
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:73" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:73" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:73" ht="60" customHeight="1">
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:73" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:73" ht="15.75">
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:73" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:73" ht="84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:73" ht="99">
       <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:73" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:73" ht="15.75">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:73" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:73" ht="67.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:73" ht="82.5">
       <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:73" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:73" ht="15.75">
       <c r="B16" s="13"/>
     </row>
-    <row r="17" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="84" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" ht="82.5">
       <c r="B18" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="15.75">
       <c r="B19" s="13"/>
     </row>
-    <row r="20" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="18"/>
     </row>
-    <row r="21" spans="2:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="102.75" customHeight="1">
       <c r="B21" s="17"/>
     </row>
   </sheetData>
@@ -3301,7 +3340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B16"/>
@@ -3310,13 +3349,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23.1" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -3324,91 +3363,91 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="61.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="61.35" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="65.099999999999994" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="60.6" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" ht="59.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="59.1" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="59.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="59.1" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="57.6" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="57" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="53.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="53.65" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="53.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="53.65" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="50.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="50.65" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="50.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="50.65" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="47.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="47.1" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="48" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="51.6" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="50.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="50.65" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>

</xml_diff>